<commit_message>
fix purchase/sales order resource/table/fields;
</commit_message>
<xml_diff>
--- a/public/templates/goods.xlsx
+++ b/public/templates/goods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangxiaopei/work/huayan2/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3AE6AB-1884-F34A-9236-58E54FD3EC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821D55FE-B013-384F-A658-35D47468A705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" xr2:uid="{318EE4C6-ECB0-EE48-905F-0535CD2B463E}"/>
+    <workbookView xWindow="1560" yWindow="1380" windowWidth="27240" windowHeight="14940" xr2:uid="{318EE4C6-ECB0-EE48-905F-0535CD2B463E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,29 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
-  <si>
-    <t>家富康A型足浴盆</t>
-  </si>
-  <si>
-    <t>电子产品</t>
-  </si>
-  <si>
-    <t>大华</t>
-  </si>
-  <si>
-    <t>家富康</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>上架</t>
   </si>
   <si>
-    <t>家富康B型足浴盆</t>
-  </si>
-  <si>
-    <t>福康</t>
-  </si>
-  <si>
     <t>库存</t>
   </si>
   <si>
@@ -82,25 +64,58 @@
   </si>
   <si>
     <t>价格</t>
+  </si>
+  <si>
+    <t>营养</t>
+  </si>
+  <si>
+    <t>新新健康</t>
+  </si>
+  <si>
+    <t>雀巢</t>
+  </si>
+  <si>
+    <t>保健</t>
+  </si>
+  <si>
+    <t>推荐</t>
+  </si>
+  <si>
+    <t>西麦</t>
+  </si>
+  <si>
+    <t>雀巢怡养中老年奶粉</t>
+  </si>
+  <si>
+    <t>中老年澳洲复合燕麦片700g</t>
+  </si>
+  <si>
+    <t>康恩贝维生素vc咀嚼片</t>
+  </si>
+  <si>
+    <t>康恩贝</t>
+  </si>
+  <si>
+    <t>本博颈椎按摩器按摩枕头</t>
+  </si>
+  <si>
+    <t>本博</t>
+  </si>
+  <si>
+    <t>采购价</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF3C4B5F"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -133,7 +148,9 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,97 +465,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69A92CF-7943-7648-A708-EF841FF2EC6F}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>178</v>
+      </c>
+      <c r="F2">
+        <v>239</v>
+      </c>
+      <c r="G2">
+        <v>88</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="F3">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="G3">
+        <v>6.8</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>0.02</v>
+      </c>
+      <c r="F4">
+        <v>338</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>50</v>
+      </c>
+      <c r="I4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>0.01</v>
+      </c>
+      <c r="F5">
+        <v>59</v>
+      </c>
+      <c r="G5">
+        <v>0.01</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>156</v>
-      </c>
-      <c r="F2">
-        <v>398</v>
-      </c>
-      <c r="G2">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>258</v>
-      </c>
-      <c r="F3">
-        <v>598</v>
-      </c>
-      <c r="G3">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>4</v>
-      </c>
+      <c r="J5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>